<commit_message>
Added file (Test Cases) is commiting now
</commit_message>
<xml_diff>
--- a/src/mindFullMarket/XLSfiles/Module1.xlsx
+++ b/src/mindFullMarket/XLSfiles/Module1.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18460" windowHeight="5680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14820" windowHeight="5680"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="UpdateMePopUp" sheetId="3" r:id="rId2"/>
+    <sheet name="ValidateSignIn" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Module ID</t>
   </si>
@@ -34,26 +36,56 @@
     <t>To validate User</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Extract Manufacturar discription</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>ValidateUser</t>
-  </si>
-  <si>
-    <t>ExtractManufacturar</t>
+    <t>ValidateSignIn</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Passward</t>
+  </si>
+  <si>
+    <t>jigesh@sjainfosolutions.com</t>
+  </si>
+  <si>
+    <t>aakash104</t>
+  </si>
+  <si>
+    <t>jigesh1@sjainfosolutions.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UpdateMePopUp</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>shail@solvios.technology</t>
+  </si>
+  <si>
+    <t>Shail</t>
+  </si>
+  <si>
+    <t>shail1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +97,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,15 +148,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,7 +442,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,27 +465,141 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>